<commit_message>
Script to use same logic as bulk_insert.py, but get fragments in reactants and products
</commit_message>
<xml_diff>
--- a/Neo4j/BulkChem/bulkchem_datafiles/Function-Groups-SMARTS.xlsx
+++ b/Neo4j/BulkChem/bulkchem_datafiles/Function-Groups-SMARTS.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\PycharmProjects\McQuade-Chem-ML\Neo4j\BulkChem\bulkchem_datafiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0818009E-6006-4E0B-A464-131C42124DAF}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E1C6C06-54EA-41A3-8DFC-19B750FFE693}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="74">
   <si>
     <t>Fragment</t>
   </si>
@@ -182,6 +182,66 @@
   </si>
   <si>
     <t>[$(P(=[OX1])([OX2][#6])([$([OX2H]),$([OX1-]),$([OX2][#6])])[$([OX2H]),$([OX1-]),$([OX2][#6]),$([OX2]P)]),$([P+]([OX1-])([OX2][#6])([$([OX2H]),$([OX1-]),$([OX2][#6])])[$([OX2H]),$([OX1-]),$([OX2][#6]),$([OX2]P)])]</t>
+  </si>
+  <si>
+    <t>Acetylenic Carbon</t>
+  </si>
+  <si>
+    <t>[$([CX2]#C)]</t>
+  </si>
+  <si>
+    <t>Anhydride</t>
+  </si>
+  <si>
+    <t>[CX3](=[OX1])[OX2][CX3](=[OX1])</t>
+  </si>
+  <si>
+    <t>Amidinium</t>
+  </si>
+  <si>
+    <t>[NX3][CX3]=[NX3+]</t>
+  </si>
+  <si>
+    <t>Cyanamide</t>
+  </si>
+  <si>
+    <t>[NX3][CX2]#[NX1]</t>
+  </si>
+  <si>
+    <t>Enamine</t>
+  </si>
+  <si>
+    <t>[NX3][CX3]=[CX3]</t>
+  </si>
+  <si>
+    <t>Aniline Nitrogen</t>
+  </si>
+  <si>
+    <t>[NX3][$(C=C),$(cc)]</t>
+  </si>
+  <si>
+    <t>[$(*-[NX2-]-[NX2+]#[NX1]),$(*-[NX2]=[NX2+]=[NX1-])]</t>
+  </si>
+  <si>
+    <t>Azide</t>
+  </si>
+  <si>
+    <t>[NX2]=N</t>
+  </si>
+  <si>
+    <t>Azo Nitrogen</t>
+  </si>
+  <si>
+    <t>[$([SX4](=O)(=O)(O)O),$([SX4+2]([O-])([O-])(O)O)]</t>
+  </si>
+  <si>
+    <t>Sulfuric acid</t>
+  </si>
+  <si>
+    <t>Alkyl Carbon</t>
+  </si>
+  <si>
+    <t>[CX4]</t>
   </si>
 </sst>
 </file>
@@ -1022,15 +1082,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:D34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" zoomScale="106" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="41.26953125" customWidth="1"/>
+    <col min="1" max="1" width="14.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="52" customWidth="1"/>
+    <col min="3" max="3" width="14.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
@@ -1119,133 +1181,236 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>4</v>
+        <v>64</v>
       </c>
       <c r="B7" t="s">
-        <v>5</v>
+        <v>65</v>
+      </c>
+      <c r="C7" t="s">
+        <v>62</v>
+      </c>
+      <c r="D7" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B13" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B14" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B16" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B17" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B18" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B19" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B20" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B21" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
+        <v>32</v>
+      </c>
+      <c r="B22" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
         <v>34</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B23" t="s">
         <v>35</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>54</v>
+      </c>
+      <c r="B24" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>56</v>
+      </c>
+      <c r="B25" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>58</v>
+      </c>
+      <c r="B26" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>60</v>
+      </c>
+      <c r="B27" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>67</v>
+      </c>
+      <c r="B28" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>69</v>
+      </c>
+      <c r="B29" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>71</v>
+      </c>
+      <c r="B30" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>72</v>
+      </c>
+      <c r="B31" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>18</v>
+      </c>
+      <c r="B32" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>20</v>
+      </c>
+      <c r="B33" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>54</v>
+      </c>
+      <c r="B34" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>